<commit_message>
data dictionary draft 1 done
</commit_message>
<xml_diff>
--- a/DATA_DICTONARY.xlsx
+++ b/DATA_DICTONARY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveswinburneeduau-my.sharepoint.com/personal/103615452_student_swin_edu_au/Documents/CertIV/Shared Projects/Heroes Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{7CD9155E-AEDB-43D8-B65A-3D451335CA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B231A3C-9A44-49C5-B326-377796CF5E76}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{7CD9155E-AEDB-43D8-B65A-3D451335CA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE3E4B58-B7E9-4E20-B679-93B2990A4393}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <r>
       <rPr>
@@ -48,110 +48,10 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Long description of the tour.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ClientId</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
       <t>INT</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>A sequentially assigned surrogate key e.g. 1, 2 3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Surname</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>NOT NULL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>GivenName</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gender</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>NVARCHAR(1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>CHECK IN (‘M’, ‘F’, ‘I’), (NULLABLE)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Gender, must be onbe of M, F or I</t>
-    </r>
-  </si>
-  <si>
     <t>Data Dictionary</t>
   </si>
   <si>
@@ -173,36 +73,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>StaffID</t>
-  </si>
-  <si>
-    <t>NVARCHAR(10)</t>
-  </si>
-  <si>
-    <t>Staff ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>NVACHAR(15)</t>
-  </si>
-  <si>
-    <t>Not Null</t>
-  </si>
-  <si>
-    <t>Staff Name</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>CHECK Length = 10</t>
-  </si>
-  <si>
-    <t>e.g "0494601129"</t>
-  </si>
-  <si>
     <t>Hero</t>
   </si>
   <si>
@@ -237,6 +107,51 @@
   </si>
   <si>
     <t>Minimum number dice can roll</t>
+  </si>
+  <si>
+    <t>VillainID</t>
+  </si>
+  <si>
+    <t>HitPoints</t>
+  </si>
+  <si>
+    <t>VName</t>
+  </si>
+  <si>
+    <t>A unique ID generated for each Villain</t>
+  </si>
+  <si>
+    <t>Name of the hero e.g. BADMAN</t>
+  </si>
+  <si>
+    <t>Maximum number dice can roll</t>
+  </si>
+  <si>
+    <t>Num of times a hero can be used</t>
+  </si>
+  <si>
+    <t>Villain's health</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>GameID</t>
+  </si>
+  <si>
+    <t>Game Number (so the Pkeys don’t crash with each other)</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>TurnNumber</t>
+  </si>
+  <si>
+    <t>Recording turn for each turn (hero vs villain) ALSO (so the Pkeys don’t crash with each other)</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
   </si>
 </sst>
 </file>
@@ -307,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -345,22 +260,54 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -368,13 +315,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -390,26 +334,62 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -753,7 +733,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -762,239 +742,256 @@
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="39.5" customWidth="1"/>
-    <col min="5" max="5" width="59.33203125" customWidth="1"/>
+    <col min="5" max="5" width="99" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="D7" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21"/>
+      <c r="B9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21"/>
+      <c r="B10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B12" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="22"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="2" t="s">
+      <c r="B15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="2" t="s">
+      <c r="C15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A12:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>